<commit_message>
added multi user support, captcha solving and apk downloading features
</commit_message>
<xml_diff>
--- a/src/config.xlsx
+++ b/src/config.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anon\PycharmProjects\aws_appstore_automation\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78059F58-416E-486D-9C26-CC781AC708E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC81BBE-FB20-4476-B0BD-652E055E1490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="creds" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="58">
   <si>
     <t>SN</t>
   </si>
@@ -46,27 +47,6 @@
     <t>game_features</t>
   </si>
   <si>
-    <t>static_folder_path</t>
-  </si>
-  <si>
-    <t>Doll Dress Up</t>
-  </si>
-  <si>
-    <t>Limbs Run</t>
-  </si>
-  <si>
-    <t>Fleet Manager</t>
-  </si>
-  <si>
-    <t>IronThemAll</t>
-  </si>
-  <si>
-    <t>Shot Range Run</t>
-  </si>
-  <si>
-    <t>Screw Master</t>
-  </si>
-  <si>
     <t>Games</t>
   </si>
   <si>
@@ -148,30 +128,103 @@
     <t>Multiplayer</t>
   </si>
   <si>
-    <t>C:\Users\Anon\Downloads\Compressed\Games\Games\Doll Dress Up</t>
-  </si>
-  <si>
-    <t>C:\Users\Anon\Downloads\Compressed\Games\Games\Limbs Run</t>
-  </si>
-  <si>
-    <t>C:\Users\Anon\Downloads\Compressed\Games\Games\Fleet Manager</t>
-  </si>
-  <si>
-    <t>C:\Users\Anon\Downloads\Compressed\Games\Games\IronThemAll</t>
-  </si>
-  <si>
-    <t>C:\Users\Anon\Downloads\Compressed\Games\Games\Shot Range Run</t>
-  </si>
-  <si>
-    <t>C:\Users\Anon\Downloads\Compressed\Games\Games\Screw Master</t>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>TOTP</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>amit</t>
+  </si>
+  <si>
+    <t>amit1</t>
+  </si>
+  <si>
+    <t>amit2</t>
+  </si>
+  <si>
+    <t>amit3</t>
+  </si>
+  <si>
+    <t>google_play_apk_url</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=com.sec.android.app.popupcalculator</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=com.sec.android.app.clockpackage</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=com.samsung.android.app.notes</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=notes.notepad.checklist.calendar.todolist.notebook</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=com.atomczak.notepat</t>
+  </si>
+  <si>
+    <t>pop calculator</t>
+  </si>
+  <si>
+    <t>clock</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>todo notes</t>
+  </si>
+  <si>
+    <t>notepad</t>
+  </si>
+  <si>
+    <t>password123</t>
+  </si>
+  <si>
+    <t>RUL36UYIL2KGMWFPM33YQ4VDQZIAODr3rr32r746724672374</t>
+  </si>
+  <si>
+    <t>dummy_email_1@gmail.com</t>
+  </si>
+  <si>
+    <t>dummy_email_2@gmail.com</t>
+  </si>
+  <si>
+    <t>dummy_email_3@gmail.com</t>
+  </si>
+  <si>
+    <t>dummy_email_4@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -196,13 +249,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -481,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -494,198 +551,206 @@
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="83.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" t="s">
         <v>39</v>
       </c>
-      <c r="G2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" t="s">
-        <v>45</v>
+        <v>32</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{2A06C39C-76A1-479F-85EE-DCC4C27406A8}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{F8DF85AD-7D3A-4C5D-9BEE-60EF01886101}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{132E3554-804F-44C1-9FC2-BDC1A61A28BE}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{BB9F7EB3-3018-4C1A-8C74-583509AF540F}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{94243452-45D1-433B-939D-5742039EDD6A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B392DB25-7F51-4FA3-9C2A-4204FF547DE8}">
           <x14:formula1>
             <xm:f>Sheet2!$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C50</xm:sqref>
+          <xm:sqref>C3:C49</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{05D6A7B2-4F56-43F2-8260-CBA956C08F2A}">
           <x14:formula1>
             <xm:f>Sheet2!$B$2:$B$19</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D842</xm:sqref>
+          <xm:sqref>D3:D841</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{07201D7E-F1E6-4E75-B6A7-C72EC2AD47ED}">
           <x14:formula1>
             <xm:f>Sheet2!$C$2</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E881</xm:sqref>
+          <xm:sqref>E3:E880</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{896A9EE7-C422-41B1-8E9C-C087C196AEAA}">
           <x14:formula1>
             <xm:f>Sheet2!$D$2:$D$6</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F582</xm:sqref>
+          <xm:sqref>F3:F581</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7F4737B8-35A0-4A26-B8FC-32FD9AA8A264}">
+          <x14:formula1>
+            <xm:f>creds!$B$2:$B$1048576</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -694,6 +759,122 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8135A3C7-7A62-4DC4-B294-3465A85C2CC2}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{3F1166E3-E503-472B-8316-3FC162797BAF}">
+      <formula1>COUNTIF($B:$B,B2)&lt;2</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{B98B9D7B-72F7-46AC-A01E-09F9DA563391}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{636B45AD-AF9E-42E3-A88A-20287D460AA8}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{4B98F808-FA82-4ABE-8E58-F45BF3A38073}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{8E004C73-7C86-4FBE-AB08-C6ED95D70421}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B034318-E67E-47CB-9529-5F548AEC2415}">
   <dimension ref="A1:D19"/>
   <sheetViews>
@@ -705,10 +886,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
@@ -719,116 +900,116 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
version 2 of apk automation
</commit_message>
<xml_diff>
--- a/src/config.xlsx
+++ b/src/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anon\PycharmProjects\aws_appstore_automation\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D74C482-F46E-45C0-A75C-94778114BE47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7CDD92A-B476-405A-9448-7AA3E4B14C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
   <si>
     <t>SN</t>
   </si>
@@ -47,6 +47,12 @@
     <t>google_play_apk_url</t>
   </si>
   <si>
+    <t>package_name</t>
+  </si>
+  <si>
+    <t>base_apkname</t>
+  </si>
+  <si>
     <t>username</t>
   </si>
   <si>
@@ -62,111 +68,114 @@
     <t>Multiplayer</t>
   </si>
   <si>
-    <t>https://play.google.com/store/apps/details?id=com.stickman.warriors.stickwarriors.dragon.shadow.fight</t>
+    <t>https://play.google.com/store/apps/details?id=com.hotyetistudio.eggsortpuzzle</t>
+  </si>
+  <si>
+    <t>com.maridilo.fosixgame1</t>
+  </si>
+  <si>
+    <t>emt.apk</t>
   </si>
   <si>
     <t>account1</t>
   </si>
   <si>
-    <t>https://play.google.com/store/apps/details?id=com.avatarlife.avatarstory.mystory.myworld.mywonder</t>
-  </si>
-  <si>
-    <t>https://play.google.com/store/apps/details?id=com.colorpainting.colorbook.colorasmr.coloring.drawpainting.colorpage</t>
-  </si>
-  <si>
-    <t>https://play.google.com/store/apps/details?id=com.diygame.dolldressup.dressup.makeup.anime.princess</t>
-  </si>
-  <si>
-    <t>https://play.google.com/store/apps/details?id=com.riddlephysics.trickypuzzle.brainpuzzle.braintest</t>
+    <t>https://play.google.com/store/apps/details?id=com.hotyetistudio.colorwario</t>
+  </si>
+  <si>
+    <t>com.maridilo.fosixgame2</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=com.hotyetistudio.sortadventure</t>
+  </si>
+  <si>
+    <t>com.maridilo.fosixgame3</t>
+  </si>
+  <si>
+    <t>com.maridilo.fosixgame4</t>
+  </si>
+  <si>
+    <t>account2</t>
+  </si>
+  <si>
+    <t>account3</t>
+  </si>
+  <si>
+    <t>account4</t>
+  </si>
+  <si>
+    <t>account5</t>
+  </si>
+  <si>
+    <t>account6</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>TOTP</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>sub_category</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Casual</t>
+  </si>
+  <si>
+    <t>Adventure</t>
+  </si>
+  <si>
+    <t>Indie</t>
+  </si>
+  <si>
+    <t>Live Wallpaper</t>
+  </si>
+  <si>
+    <t>Board</t>
+  </si>
+  <si>
+    <t>Widget</t>
+  </si>
+  <si>
+    <t>Brain &amp; Puzzle</t>
+  </si>
+  <si>
+    <t>Cards</t>
+  </si>
+  <si>
+    <t>Casino</t>
+  </si>
+  <si>
+    <t>Dice</t>
+  </si>
+  <si>
+    <t>Fantasy</t>
+  </si>
+  <si>
+    <t>Music &amp; Rhythm</t>
+  </si>
+  <si>
+    <t>Racing</t>
   </si>
   <si>
     <t>Role Playing</t>
   </si>
   <si>
-    <t>account2</t>
+    <t>Seek &amp; Find</t>
   </si>
   <si>
     <t>Simulation</t>
   </si>
   <si>
-    <t>account3</t>
-  </si>
-  <si>
-    <t>account4</t>
-  </si>
-  <si>
-    <t>account5</t>
-  </si>
-  <si>
-    <t>account6</t>
-  </si>
-  <si>
-    <t>account7</t>
-  </si>
-  <si>
-    <t>Adventure</t>
-  </si>
-  <si>
-    <t>account8</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>TOTP</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>sub_category</t>
-  </si>
-  <si>
-    <t>Action</t>
-  </si>
-  <si>
-    <t>Casual</t>
-  </si>
-  <si>
-    <t>Indie</t>
-  </si>
-  <si>
-    <t>Live Wallpaper</t>
-  </si>
-  <si>
-    <t>Board</t>
-  </si>
-  <si>
-    <t>Widget</t>
-  </si>
-  <si>
-    <t>Brain &amp; Puzzle</t>
-  </si>
-  <si>
-    <t>Cards</t>
-  </si>
-  <si>
-    <t>Casino</t>
-  </si>
-  <si>
-    <t>Dice</t>
-  </si>
-  <si>
-    <t>Fantasy</t>
-  </si>
-  <si>
-    <t>Music &amp; Rhythm</t>
-  </si>
-  <si>
-    <t>Racing</t>
-  </si>
-  <si>
-    <t>Seek &amp; Find</t>
-  </si>
-  <si>
     <t>Sports Games</t>
   </si>
   <si>
@@ -179,41 +188,32 @@
     <t>Words</t>
   </si>
   <si>
-    <t>package_name</t>
-  </si>
-  <si>
-    <t>com.test.amit1</t>
-  </si>
-  <si>
-    <t>com.test.amit3</t>
-  </si>
-  <si>
-    <t>com.test.amit4</t>
-  </si>
-  <si>
-    <t>com.test.amit5</t>
-  </si>
-  <si>
-    <t>com.test.amit6</t>
-  </si>
-  <si>
-    <t>base_apkname</t>
-  </si>
-  <si>
-    <t>test.apk</t>
+    <t>test@gmail.com</t>
   </si>
   <si>
     <t>test1@gmail.com</t>
   </si>
   <si>
-    <t>abc</t>
+    <t>test3@outlook.com</t>
+  </si>
+  <si>
+    <t>test4@yahoo.com</t>
+  </si>
+  <si>
+    <t>test7@gmail.com</t>
+  </si>
+  <si>
+    <t>tes1@gmail.com</t>
+  </si>
+  <si>
+    <t>gfhsieyytytyytyt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,22 +255,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -306,12 +305,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -320,10 +349,15 @@
       <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -607,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -644,42 +678,42 @@
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -687,28 +721,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -716,28 +750,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -745,66 +779,40 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" t="s">
         <v>15</v>
       </c>
-      <c r="G5" t="s">
-        <v>54</v>
-      </c>
-      <c r="H5" t="s">
-        <v>57</v>
-      </c>
       <c r="I5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
         <v>16</v>
-      </c>
-      <c r="G6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" t="s">
-        <v>57</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I6" xr:uid="{3B2DE811-CC67-40CD-97B5-47F45BF137FB}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I5" xr:uid="{3B2DE811-CC67-40CD-97B5-47F45BF137FB}">
       <formula1>COUNTIF($B:$B,I2)&lt;2</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{8241A8F2-EAE3-41BB-A953-82335CDD3BCC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -813,7 +821,7 @@
           <x14:formula1>
             <xm:f>creds!$B$2:$B$1048576</xm:f>
           </x14:formula1>
-          <xm:sqref>I7:I1048576</xm:sqref>
+          <xm:sqref>I6:I1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -823,10 +831,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8135A3C7-7A62-4DC4-B294-3465A85C2CC2}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -842,7 +850,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>27</v>
@@ -859,134 +867,100 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="7">
+        <v>1234</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="7">
+        <v>1234</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1234</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="7">
+        <v>1234</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="7">
+        <v>1234</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D7" s="7">
         <v>1234</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="4">
-        <v>1234</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" s="4">
-        <v>1234</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" s="4">
-        <v>1234</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="4">
-        <v>1234</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="4">
-        <v>1234</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" s="4">
-        <v>1234</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="4">
-        <v>1234</v>
-      </c>
-      <c r="E9" s="6" t="s">
+      <c r="E7" s="4" t="s">
         <v>59</v>
       </c>
     </row>
@@ -997,8 +971,12 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{1C43488D-080F-4B02-941B-A19ED10955DF}"/>
-    <hyperlink ref="C3:C9" r:id="rId2" display="test1@gmail.com" xr:uid="{DA73B2EA-8B38-4CB5-B8A6-6D79D0F3B2F1}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{382B9779-7BFA-4463-8F88-A286A1BEBE2F}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{6DCA3372-9F70-4103-93A6-345B44C0F83F}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{04E03B50-8CCD-45C1-BE10-42FF62D56EED}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{91D8C2B5-C110-45C4-B765-5821D86F20F8}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{B48FB2C0-7554-46A8-B83A-D98591F1D76F}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{72D54A9B-AD69-4E15-9634-6028EECEB548}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1030,13 +1008,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
         <v>33</v>
@@ -1044,102 +1022,102 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added ui for the automation script
</commit_message>
<xml_diff>
--- a/src/config.xlsx
+++ b/src/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anon\PycharmProjects\aws_appstore_automation\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7CDD92A-B476-405A-9448-7AA3E4B14C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC6E1110-566B-4138-A93C-25ABA762579C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11085" yWindow="-14745" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
   <si>
     <t>SN</t>
   </si>
@@ -50,170 +50,119 @@
     <t>package_name</t>
   </si>
   <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>Games</t>
+  </si>
+  <si>
+    <t>Simulation</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Multiplayer</t>
+  </si>
+  <si>
+    <t>account1</t>
+  </si>
+  <si>
+    <t>https://play.google.com/store/apps/details?id=com.tocaboca.tocalifeworld</t>
+  </si>
+  <si>
+    <t>com.asdevmat.croc4</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>TOTP</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>sub_category</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Casual</t>
+  </si>
+  <si>
+    <t>Adventure</t>
+  </si>
+  <si>
+    <t>Indie</t>
+  </si>
+  <si>
+    <t>Arcade</t>
+  </si>
+  <si>
+    <t>Live Wallpaper</t>
+  </si>
+  <si>
+    <t>Board</t>
+  </si>
+  <si>
+    <t>Widget</t>
+  </si>
+  <si>
+    <t>Brain &amp; Puzzle</t>
+  </si>
+  <si>
+    <t>Cards</t>
+  </si>
+  <si>
+    <t>Casino</t>
+  </si>
+  <si>
+    <t>Dice</t>
+  </si>
+  <si>
+    <t>Fantasy</t>
+  </si>
+  <si>
+    <t>Music &amp; Rhythm</t>
+  </si>
+  <si>
+    <t>Racing</t>
+  </si>
+  <si>
+    <t>Role Playing</t>
+  </si>
+  <si>
+    <t>Seek &amp; Find</t>
+  </si>
+  <si>
+    <t>Sports Games</t>
+  </si>
+  <si>
+    <t>Strategy</t>
+  </si>
+  <si>
+    <t>Trivia</t>
+  </si>
+  <si>
+    <t>Words</t>
+  </si>
+  <si>
     <t>base_apkname</t>
   </si>
   <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>Games</t>
-  </si>
-  <si>
-    <t>Arcade</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>Multiplayer</t>
-  </si>
-  <si>
-    <t>https://play.google.com/store/apps/details?id=com.hotyetistudio.eggsortpuzzle</t>
-  </si>
-  <si>
-    <t>com.maridilo.fosixgame1</t>
-  </si>
-  <si>
     <t>emt.apk</t>
-  </si>
-  <si>
-    <t>account1</t>
-  </si>
-  <si>
-    <t>https://play.google.com/store/apps/details?id=com.hotyetistudio.colorwario</t>
-  </si>
-  <si>
-    <t>com.maridilo.fosixgame2</t>
-  </si>
-  <si>
-    <t>https://play.google.com/store/apps/details?id=com.hotyetistudio.sortadventure</t>
-  </si>
-  <si>
-    <t>com.maridilo.fosixgame3</t>
-  </si>
-  <si>
-    <t>com.maridilo.fosixgame4</t>
-  </si>
-  <si>
-    <t>account2</t>
-  </si>
-  <si>
-    <t>account3</t>
-  </si>
-  <si>
-    <t>account4</t>
-  </si>
-  <si>
-    <t>account5</t>
-  </si>
-  <si>
-    <t>account6</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>TOTP</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>sub_category</t>
-  </si>
-  <si>
-    <t>Action</t>
-  </si>
-  <si>
-    <t>Casual</t>
-  </si>
-  <si>
-    <t>Adventure</t>
-  </si>
-  <si>
-    <t>Indie</t>
-  </si>
-  <si>
-    <t>Live Wallpaper</t>
-  </si>
-  <si>
-    <t>Board</t>
-  </si>
-  <si>
-    <t>Widget</t>
-  </si>
-  <si>
-    <t>Brain &amp; Puzzle</t>
-  </si>
-  <si>
-    <t>Cards</t>
-  </si>
-  <si>
-    <t>Casino</t>
-  </si>
-  <si>
-    <t>Dice</t>
-  </si>
-  <si>
-    <t>Fantasy</t>
-  </si>
-  <si>
-    <t>Music &amp; Rhythm</t>
-  </si>
-  <si>
-    <t>Racing</t>
-  </si>
-  <si>
-    <t>Role Playing</t>
-  </si>
-  <si>
-    <t>Seek &amp; Find</t>
-  </si>
-  <si>
-    <t>Simulation</t>
-  </si>
-  <si>
-    <t>Sports Games</t>
-  </si>
-  <si>
-    <t>Strategy</t>
-  </si>
-  <si>
-    <t>Trivia</t>
-  </si>
-  <si>
-    <t>Words</t>
-  </si>
-  <si>
-    <t>test@gmail.com</t>
-  </si>
-  <si>
-    <t>test1@gmail.com</t>
-  </si>
-  <si>
-    <t>test3@outlook.com</t>
-  </si>
-  <si>
-    <t>test4@yahoo.com</t>
-  </si>
-  <si>
-    <t>test7@gmail.com</t>
-  </si>
-  <si>
-    <t>tes1@gmail.com</t>
-  </si>
-  <si>
-    <t>gfhsieyytytyytyt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,11 +204,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -269,7 +213,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -305,42 +249,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -349,15 +263,7 @@
       <alignment readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -641,19 +547,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="101.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="63.44140625" customWidth="1"/>
     <col min="7" max="8" width="24.6640625" customWidth="1"/>
     <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -681,160 +588,59 @@
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I5" xr:uid="{3B2DE811-CC67-40CD-97B5-47F45BF137FB}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{0EC52FDE-9681-496C-9986-9C1B19731AE6}">
       <formula1>COUNTIF($B:$B,I2)&lt;2</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{8241A8F2-EAE3-41BB-A953-82335CDD3BCC}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7F4737B8-35A0-4A26-B8FC-32FD9AA8A264}">
-          <x14:formula1>
-            <xm:f>creds!$B$2:$B$1048576</xm:f>
-          </x14:formula1>
-          <xm:sqref>I6:I1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8135A3C7-7A62-4DC4-B294-3465A85C2CC2}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -850,119 +656,157 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="7">
-        <v>1234</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>59</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="7">
-        <v>1234</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>59</v>
-      </c>
+      <c r="A3" s="2"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="8">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4" s="7">
-        <v>1234</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>59</v>
-      </c>
+      <c r="A4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="8">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" s="7">
-        <v>1234</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>59</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="8">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D6" s="7">
-        <v>1234</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>59</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="8">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="7">
-        <v>1234</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>59</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="2"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="2"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -970,14 +814,6 @@
       <formula1>COUNTIF($B:$B,B2)&lt;2</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{382B9779-7BFA-4463-8F88-A286A1BEBE2F}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{6DCA3372-9F70-4103-93A6-345B44C0F83F}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{04E03B50-8CCD-45C1-BE10-42FF62D56EED}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{91D8C2B5-C110-45C4-B765-5821D86F20F8}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{B48FB2C0-7554-46A8-B83A-D98591F1D76F}"/>
-    <hyperlink ref="C7" r:id="rId6" xr:uid="{72D54A9B-AD69-4E15-9634-6028EECEB548}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -994,10 +830,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -1008,116 +844,116 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>